<commit_message>
MAJ des HDV c794c599cd92a206d9ab94c6cb0b06401bef4a30
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-ActorXDS.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-ActorXDS.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-05T11:54:16+00:00</t>
+    <t>2025-05-05T14:17:01+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,8 @@
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Cet attribut représente un acteur (humain ou système) ayant contribué au document. Pour les documents d’expression personnelle du patient, cette métadonnée fait référence au patient. </t>
+    <t>Cet attribut représente un acteur (humain ou système) ayant contribué au document. Pour les documents d’expression personnelle du patient, cette métadonnée fait référence au patient. 
+XCN de HL7 v2.5</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>